<commit_message>
Zusammenführen und vereinheitlichen der AP
Arbeitspakete sind zusammengefasst, des weiteren wurden alle älteren versionen der AP in einem neuen Ordner (Historie AP) abgelegt. Desweiteren wurden andere dateien auch sortieret.
</commit_message>
<xml_diff>
--- a/Abgabe 23.06.2025/Gantt-Chart.xlsx
+++ b/Abgabe 23.06.2025/Gantt-Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\github projektrealisierung\Abgabe 23.06.2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B5F5FC-AEB8-4A0C-8377-C0E65F79F6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EE57B2-E78E-4649-AF4A-6C53F2B23743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AABDB1AC-CD74-4E1B-8EC2-2681E98F722A}"/>
   </bookViews>
@@ -647,9 +647,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="dd/mm/"/>
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1399,13 +1399,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -1417,7 +1417,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1468,7 +1468,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1490,7 +1490,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
@@ -1508,7 +1508,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1535,141 +1535,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1679,28 +1544,24 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1715,14 +1576,149 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1829,7 +1825,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
+      <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3174,10 +3170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552E000D-C45B-4C4B-998B-9AC71E5E90DD}">
-  <dimension ref="A1:CE55"/>
+  <dimension ref="A1:CD55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3198,40 +3194,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="128" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
     </row>
     <row r="2" spans="1:82" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:82" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="124"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="74" t="s">
         <v>21</v>
       </c>
       <c r="I3"/>
@@ -3240,23 +3236,23 @@
       <c r="B4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="78" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="21"/>
-      <c r="E4" s="129" t="s">
+      <c r="E4" s="82" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="126" t="s">
+      <c r="C5" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="130" t="s">
+      <c r="E5" s="83" t="s">
         <v>29</v>
       </c>
       <c r="I5"/>
@@ -3268,10 +3264,10 @@
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="127">
+      <c r="C6" s="80">
         <v>45786</v>
       </c>
-      <c r="E6" s="130" t="s">
+      <c r="E6" s="83" t="s">
         <v>30</v>
       </c>
       <c r="I6"/>
@@ -3280,133 +3276,133 @@
       <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="128">
+      <c r="C7" s="81">
         <v>45849</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="84" t="s">
         <v>31</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:82" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="132" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="85" t="s">
         <v>32</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="122"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
       <c r="H9" s="22"/>
       <c r="L9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="74">
+      <c r="M9" s="121">
         <v>19</v>
       </c>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="74">
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
+      <c r="T9" s="121">
         <v>20</v>
       </c>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="74"/>
-      <c r="X9" s="74"/>
-      <c r="Y9" s="74"/>
-      <c r="Z9" s="74"/>
-      <c r="AA9" s="74">
+      <c r="U9" s="121"/>
+      <c r="V9" s="121"/>
+      <c r="W9" s="121"/>
+      <c r="X9" s="121"/>
+      <c r="Y9" s="121"/>
+      <c r="Z9" s="121"/>
+      <c r="AA9" s="121">
         <v>21</v>
       </c>
-      <c r="AB9" s="74"/>
-      <c r="AC9" s="74"/>
-      <c r="AD9" s="74"/>
-      <c r="AE9" s="74"/>
-      <c r="AF9" s="74"/>
-      <c r="AG9" s="74"/>
-      <c r="AH9" s="74">
+      <c r="AB9" s="121"/>
+      <c r="AC9" s="121"/>
+      <c r="AD9" s="121"/>
+      <c r="AE9" s="121"/>
+      <c r="AF9" s="121"/>
+      <c r="AG9" s="121"/>
+      <c r="AH9" s="121">
         <v>22</v>
       </c>
-      <c r="AI9" s="74"/>
-      <c r="AJ9" s="74"/>
-      <c r="AK9" s="74"/>
-      <c r="AL9" s="74"/>
-      <c r="AM9" s="74"/>
-      <c r="AN9" s="74"/>
-      <c r="AO9" s="74">
+      <c r="AI9" s="121"/>
+      <c r="AJ9" s="121"/>
+      <c r="AK9" s="121"/>
+      <c r="AL9" s="121"/>
+      <c r="AM9" s="121"/>
+      <c r="AN9" s="121"/>
+      <c r="AO9" s="121">
         <v>23</v>
       </c>
-      <c r="AP9" s="74"/>
-      <c r="AQ9" s="74"/>
-      <c r="AR9" s="74"/>
-      <c r="AS9" s="74"/>
-      <c r="AT9" s="74"/>
-      <c r="AU9" s="74"/>
-      <c r="AV9" s="74">
+      <c r="AP9" s="121"/>
+      <c r="AQ9" s="121"/>
+      <c r="AR9" s="121"/>
+      <c r="AS9" s="121"/>
+      <c r="AT9" s="121"/>
+      <c r="AU9" s="121"/>
+      <c r="AV9" s="121">
         <v>24</v>
       </c>
-      <c r="AW9" s="74"/>
-      <c r="AX9" s="74"/>
-      <c r="AY9" s="74"/>
-      <c r="AZ9" s="74"/>
-      <c r="BA9" s="74"/>
-      <c r="BB9" s="74"/>
-      <c r="BC9" s="74">
+      <c r="AW9" s="121"/>
+      <c r="AX9" s="121"/>
+      <c r="AY9" s="121"/>
+      <c r="AZ9" s="121"/>
+      <c r="BA9" s="121"/>
+      <c r="BB9" s="121"/>
+      <c r="BC9" s="121">
         <v>25</v>
       </c>
-      <c r="BD9" s="74"/>
-      <c r="BE9" s="74"/>
-      <c r="BF9" s="74"/>
-      <c r="BG9" s="74"/>
-      <c r="BH9" s="74"/>
-      <c r="BI9" s="74"/>
-      <c r="BJ9" s="74">
+      <c r="BD9" s="121"/>
+      <c r="BE9" s="121"/>
+      <c r="BF9" s="121"/>
+      <c r="BG9" s="121"/>
+      <c r="BH9" s="121"/>
+      <c r="BI9" s="121"/>
+      <c r="BJ9" s="121">
         <v>26</v>
       </c>
-      <c r="BK9" s="74"/>
-      <c r="BL9" s="74"/>
-      <c r="BM9" s="74"/>
-      <c r="BN9" s="74"/>
-      <c r="BO9" s="74"/>
-      <c r="BP9" s="74"/>
-      <c r="BQ9" s="74">
+      <c r="BK9" s="121"/>
+      <c r="BL9" s="121"/>
+      <c r="BM9" s="121"/>
+      <c r="BN9" s="121"/>
+      <c r="BO9" s="121"/>
+      <c r="BP9" s="121"/>
+      <c r="BQ9" s="121">
         <v>27</v>
       </c>
-      <c r="BR9" s="74"/>
-      <c r="BS9" s="74"/>
-      <c r="BT9" s="74"/>
-      <c r="BU9" s="74"/>
-      <c r="BV9" s="74"/>
-      <c r="BW9" s="74"/>
-      <c r="BX9" s="74">
+      <c r="BR9" s="121"/>
+      <c r="BS9" s="121"/>
+      <c r="BT9" s="121"/>
+      <c r="BU9" s="121"/>
+      <c r="BV9" s="121"/>
+      <c r="BW9" s="121"/>
+      <c r="BX9" s="121">
         <v>28</v>
       </c>
-      <c r="BY9" s="74"/>
-      <c r="BZ9" s="74"/>
-      <c r="CA9" s="74"/>
-      <c r="CB9" s="74"/>
-      <c r="CC9" s="74"/>
-      <c r="CD9" s="74"/>
+      <c r="BY9" s="121"/>
+      <c r="BZ9" s="121"/>
+      <c r="CA9" s="121"/>
+      <c r="CB9" s="121"/>
+      <c r="CC9" s="121"/>
+      <c r="CD9" s="121"/>
     </row>
     <row r="10" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B10" s="121"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="22"/>
       <c r="L10" s="35" t="s">
         <v>8</v>
@@ -3839,17 +3835,17 @@
       </c>
     </row>
     <row r="12" spans="1:82" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="113"/>
+      <c r="C12" s="105"/>
       <c r="D12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="71"/>
+      <c r="F12" s="125"/>
       <c r="G12" s="33" t="s">
         <v>6</v>
       </c>
@@ -3862,10 +3858,10 @@
       <c r="J12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="73"/>
+      <c r="L12" s="127"/>
       <c r="M12" s="37"/>
       <c r="N12" s="38"/>
       <c r="O12" s="38"/>
@@ -3938,19 +3934,19 @@
       <c r="CD12" s="38"/>
     </row>
     <row r="13" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="88"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="27">
         <v>1</v>
       </c>
-      <c r="E13" s="82"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="134">
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
+      <c r="G13" s="86">
         <v>45786</v>
       </c>
-      <c r="H13" s="135">
+      <c r="H13" s="87">
         <v>45800</v>
       </c>
       <c r="I13" s="31">
@@ -3959,29 +3955,29 @@
       </c>
       <c r="J13" s="31">
         <f>SUM(J14:J20)</f>
-        <v>31</v>
-      </c>
-      <c r="K13" s="95"/>
-      <c r="L13" s="99"/>
+        <v>29</v>
+      </c>
+      <c r="K13" s="116"/>
+      <c r="L13" s="111"/>
       <c r="M13" s="20"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="115"/>
-      <c r="R13" s="115"/>
-      <c r="S13" s="115"/>
-      <c r="T13" s="115"/>
-      <c r="U13" s="115"/>
-      <c r="V13" s="115"/>
-      <c r="W13" s="115"/>
-      <c r="X13" s="115"/>
-      <c r="Y13" s="115"/>
-      <c r="Z13" s="115"/>
-      <c r="AA13" s="115"/>
-      <c r="AB13" s="115"/>
-      <c r="AC13" s="115"/>
-      <c r="AD13" s="115"/>
-      <c r="AE13" s="115"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
+      <c r="S13" s="70"/>
+      <c r="T13" s="70"/>
+      <c r="U13" s="70"/>
+      <c r="V13" s="70"/>
+      <c r="W13" s="70"/>
+      <c r="X13" s="70"/>
+      <c r="Y13" s="70"/>
+      <c r="Z13" s="70"/>
+      <c r="AA13" s="70"/>
+      <c r="AB13" s="70"/>
+      <c r="AC13" s="70"/>
+      <c r="AD13" s="70"/>
+      <c r="AE13" s="70"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="11"/>
       <c r="AH13" s="11"/>
@@ -4035,15 +4031,15 @@
       <c r="CD13" s="11"/>
     </row>
     <row r="14" spans="1:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="89"/>
-      <c r="C14" s="90"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="98"/>
       <c r="D14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="111" t="s">
+      <c r="E14" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="F14" s="85"/>
+      <c r="F14" s="103"/>
       <c r="G14" s="5" t="s">
         <v>93</v>
       </c>
@@ -4056,10 +4052,10 @@
       <c r="J14" s="26">
         <v>0</v>
       </c>
-      <c r="K14" s="100" t="s">
+      <c r="K14" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="L14" s="101"/>
+      <c r="L14" s="106"/>
       <c r="M14" s="12"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -4132,15 +4128,15 @@
       <c r="CD14" s="4"/>
     </row>
     <row r="15" spans="1:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="132" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="85"/>
+      <c r="F15" s="103"/>
       <c r="G15" s="40" t="s">
         <v>93</v>
       </c>
@@ -4153,10 +4149,10 @@
       <c r="J15" s="26">
         <v>0</v>
       </c>
-      <c r="K15" s="80" t="s">
+      <c r="K15" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="L15" s="81"/>
+      <c r="L15" s="101"/>
       <c r="M15" s="12"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -4229,15 +4225,15 @@
       <c r="CD15" s="4"/>
     </row>
     <row r="16" spans="1:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="89"/>
-      <c r="C16" s="90"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
       <c r="D16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="80" t="s">
+      <c r="E16" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="86"/>
+      <c r="F16" s="92"/>
       <c r="G16" s="40" t="s">
         <v>93</v>
       </c>
@@ -4250,10 +4246,10 @@
       <c r="J16" s="26">
         <v>10</v>
       </c>
-      <c r="K16" s="80" t="s">
+      <c r="K16" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="81"/>
+      <c r="L16" s="101"/>
       <c r="M16" s="12"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -4326,15 +4322,15 @@
       <c r="CD16" s="4"/>
     </row>
     <row r="17" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="98"/>
       <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="86" t="s">
+      <c r="E17" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="40" t="s">
         <v>147</v>
       </c>
@@ -4345,20 +4341,20 @@
         <v>1</v>
       </c>
       <c r="J17" s="26">
-        <v>5</v>
-      </c>
-      <c r="K17" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="101"/>
+      <c r="L17" s="106"/>
       <c r="M17" s="12"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
       <c r="U17" s="53"/>
       <c r="V17" s="53"/>
       <c r="W17" s="53"/>
@@ -4423,15 +4419,15 @@
       <c r="CD17" s="4"/>
     </row>
     <row r="18" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="98"/>
       <c r="D18" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="86"/>
+      <c r="F18" s="92"/>
       <c r="G18" s="42" t="s">
         <v>94</v>
       </c>
@@ -4444,10 +4440,10 @@
       <c r="J18" s="7">
         <v>4</v>
       </c>
-      <c r="K18" s="80" t="s">
+      <c r="K18" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="81"/>
+      <c r="L18" s="101"/>
       <c r="M18" s="39"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -4520,15 +4516,15 @@
       <c r="CD18" s="16"/>
     </row>
     <row r="19" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="86"/>
+      <c r="F19" s="92"/>
       <c r="G19" s="42" t="s">
         <v>93</v>
       </c>
@@ -4541,10 +4537,10 @@
       <c r="J19" s="7">
         <v>8</v>
       </c>
-      <c r="K19" s="80" t="s">
+      <c r="K19" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="L19" s="81"/>
+      <c r="L19" s="101"/>
       <c r="M19" s="39"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
@@ -4617,15 +4613,15 @@
       <c r="CD19" s="16"/>
     </row>
     <row r="20" spans="2:82" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="91"/>
-      <c r="C20" s="92"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="77"/>
+      <c r="F20" s="129"/>
       <c r="G20" s="42" t="s">
         <v>94</v>
       </c>
@@ -4638,10 +4634,10 @@
       <c r="J20" s="7">
         <v>4</v>
       </c>
-      <c r="K20" s="78" t="s">
+      <c r="K20" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="L20" s="79"/>
+      <c r="L20" s="114"/>
       <c r="M20" s="39"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -4714,15 +4710,15 @@
       <c r="CD20" s="16"/>
     </row>
     <row r="21" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="88"/>
+      <c r="C21" s="96"/>
       <c r="D21" s="30">
         <v>2</v>
       </c>
-      <c r="E21" s="94"/>
-      <c r="F21" s="95"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="116"/>
       <c r="G21" s="28"/>
       <c r="H21" s="29"/>
       <c r="I21" s="32">
@@ -4733,8 +4729,8 @@
         <f>SUM(J22:J31)</f>
         <v>53</v>
       </c>
-      <c r="K21" s="95"/>
-      <c r="L21" s="99"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="111"/>
       <c r="M21" s="20"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
@@ -4746,52 +4742,52 @@
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
-      <c r="X21" s="115"/>
-      <c r="Y21" s="115"/>
-      <c r="Z21" s="115"/>
-      <c r="AA21" s="115"/>
-      <c r="AB21" s="115"/>
-      <c r="AC21" s="115"/>
-      <c r="AD21" s="115"/>
-      <c r="AE21" s="115"/>
-      <c r="AF21" s="115"/>
-      <c r="AG21" s="115"/>
-      <c r="AH21" s="115"/>
-      <c r="AI21" s="115"/>
-      <c r="AJ21" s="115"/>
-      <c r="AK21" s="115"/>
-      <c r="AL21" s="115"/>
-      <c r="AM21" s="115"/>
-      <c r="AN21" s="115"/>
-      <c r="AO21" s="115"/>
-      <c r="AP21" s="115"/>
-      <c r="AQ21" s="115"/>
-      <c r="AR21" s="115"/>
-      <c r="AS21" s="115"/>
-      <c r="AT21" s="115"/>
-      <c r="AU21" s="115"/>
-      <c r="AV21" s="115"/>
-      <c r="AW21" s="115"/>
-      <c r="AX21" s="115"/>
-      <c r="AY21" s="115"/>
-      <c r="AZ21" s="115"/>
-      <c r="BA21" s="115"/>
-      <c r="BB21" s="115"/>
-      <c r="BC21" s="115"/>
-      <c r="BD21" s="115"/>
-      <c r="BE21" s="115"/>
-      <c r="BF21" s="115"/>
-      <c r="BG21" s="115"/>
-      <c r="BH21" s="115"/>
-      <c r="BI21" s="115"/>
-      <c r="BJ21" s="115"/>
-      <c r="BK21" s="115"/>
-      <c r="BL21" s="115"/>
-      <c r="BM21" s="115"/>
-      <c r="BN21" s="115"/>
-      <c r="BO21" s="115"/>
-      <c r="BP21" s="115"/>
-      <c r="BQ21" s="115"/>
+      <c r="X21" s="70"/>
+      <c r="Y21" s="70"/>
+      <c r="Z21" s="70"/>
+      <c r="AA21" s="70"/>
+      <c r="AB21" s="70"/>
+      <c r="AC21" s="70"/>
+      <c r="AD21" s="70"/>
+      <c r="AE21" s="70"/>
+      <c r="AF21" s="70"/>
+      <c r="AG21" s="70"/>
+      <c r="AH21" s="70"/>
+      <c r="AI21" s="70"/>
+      <c r="AJ21" s="70"/>
+      <c r="AK21" s="70"/>
+      <c r="AL21" s="70"/>
+      <c r="AM21" s="70"/>
+      <c r="AN21" s="70"/>
+      <c r="AO21" s="70"/>
+      <c r="AP21" s="70"/>
+      <c r="AQ21" s="70"/>
+      <c r="AR21" s="70"/>
+      <c r="AS21" s="70"/>
+      <c r="AT21" s="70"/>
+      <c r="AU21" s="70"/>
+      <c r="AV21" s="70"/>
+      <c r="AW21" s="70"/>
+      <c r="AX21" s="70"/>
+      <c r="AY21" s="70"/>
+      <c r="AZ21" s="70"/>
+      <c r="BA21" s="70"/>
+      <c r="BB21" s="70"/>
+      <c r="BC21" s="70"/>
+      <c r="BD21" s="70"/>
+      <c r="BE21" s="70"/>
+      <c r="BF21" s="70"/>
+      <c r="BG21" s="70"/>
+      <c r="BH21" s="70"/>
+      <c r="BI21" s="70"/>
+      <c r="BJ21" s="70"/>
+      <c r="BK21" s="70"/>
+      <c r="BL21" s="70"/>
+      <c r="BM21" s="70"/>
+      <c r="BN21" s="70"/>
+      <c r="BO21" s="70"/>
+      <c r="BP21" s="70"/>
+      <c r="BQ21" s="70"/>
       <c r="BR21" s="11"/>
       <c r="BS21" s="11"/>
       <c r="BT21" s="11"/>
@@ -4807,15 +4803,15 @@
       <c r="CD21" s="11"/>
     </row>
     <row r="22" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="98"/>
       <c r="D22" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="110" t="s">
+      <c r="E22" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="96"/>
+      <c r="F22" s="94"/>
       <c r="G22" s="43" t="s">
         <v>94</v>
       </c>
@@ -4828,10 +4824,10 @@
       <c r="J22" s="6">
         <v>2</v>
       </c>
-      <c r="K22" s="80" t="s">
+      <c r="K22" s="88" t="s">
         <v>159</v>
       </c>
-      <c r="L22" s="104"/>
+      <c r="L22" s="89"/>
       <c r="M22" s="12"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -4904,15 +4900,15 @@
       <c r="CD22" s="4"/>
     </row>
     <row r="23" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="96" t="s">
+      <c r="E23" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="85"/>
+      <c r="F23" s="103"/>
       <c r="G23" s="40" t="s">
         <v>96</v>
       </c>
@@ -4925,10 +4921,10 @@
       <c r="J23" s="26">
         <v>3</v>
       </c>
-      <c r="K23" s="80" t="s">
+      <c r="K23" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="L23" s="104"/>
+      <c r="L23" s="89"/>
       <c r="M23" s="12"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -5001,15 +4997,15 @@
       <c r="CD23" s="4"/>
     </row>
     <row r="24" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="98"/>
       <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="96" t="s">
+      <c r="E24" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="85"/>
+      <c r="F24" s="103"/>
       <c r="G24" s="40" t="s">
         <v>118</v>
       </c>
@@ -5022,10 +5018,10 @@
       <c r="J24" s="26">
         <v>0</v>
       </c>
-      <c r="K24" s="100" t="s">
+      <c r="K24" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="L24" s="101"/>
+      <c r="L24" s="106"/>
       <c r="M24" s="12"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -5098,15 +5094,15 @@
       <c r="CD24" s="4"/>
     </row>
     <row r="25" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="80" t="s">
+      <c r="E25" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="96"/>
+      <c r="F25" s="94"/>
       <c r="G25" s="42" t="s">
         <v>96</v>
       </c>
@@ -5119,10 +5115,10 @@
       <c r="J25" s="7">
         <v>2</v>
       </c>
-      <c r="K25" s="80" t="s">
+      <c r="K25" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="L25" s="81"/>
+      <c r="L25" s="101"/>
       <c r="M25" s="12"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -5195,15 +5191,15 @@
       <c r="CD25" s="4"/>
     </row>
     <row r="26" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="80" t="s">
+      <c r="E26" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="86"/>
+      <c r="F26" s="92"/>
       <c r="G26" s="42" t="s">
         <v>150</v>
       </c>
@@ -5216,10 +5212,10 @@
       <c r="J26" s="7">
         <v>1</v>
       </c>
-      <c r="K26" s="80" t="s">
+      <c r="K26" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="L26" s="104"/>
+      <c r="L26" s="89"/>
       <c r="M26" s="39"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
@@ -5292,15 +5288,15 @@
       <c r="CD26" s="16"/>
     </row>
     <row r="27" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="98"/>
       <c r="D27" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="80" t="s">
+      <c r="E27" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="86"/>
+      <c r="F27" s="92"/>
       <c r="G27" s="42" t="s">
         <v>128</v>
       </c>
@@ -5313,10 +5309,10 @@
       <c r="J27" s="7">
         <v>3</v>
       </c>
-      <c r="K27" s="80" t="s">
+      <c r="K27" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="104"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="39"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -5389,15 +5385,15 @@
       <c r="CD27" s="16"/>
     </row>
     <row r="28" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="98"/>
       <c r="D28" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="80" t="s">
+      <c r="E28" s="88" t="s">
         <v>165</v>
       </c>
-      <c r="F28" s="86"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="42" t="s">
         <v>102</v>
       </c>
@@ -5410,10 +5406,10 @@
       <c r="J28" s="7">
         <v>13</v>
       </c>
-      <c r="K28" s="80" t="s">
+      <c r="K28" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="L28" s="104"/>
+      <c r="L28" s="89"/>
       <c r="M28" s="39"/>
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
@@ -5486,15 +5482,15 @@
       <c r="CD28" s="16"/>
     </row>
     <row r="29" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="98"/>
       <c r="D29" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="F29" s="86"/>
+      <c r="F29" s="92"/>
       <c r="G29" s="42" t="s">
         <v>125</v>
       </c>
@@ -5507,10 +5503,10 @@
       <c r="J29" s="7">
         <v>2</v>
       </c>
-      <c r="K29" s="85" t="s">
+      <c r="K29" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="L29" s="101"/>
+      <c r="L29" s="106"/>
       <c r="M29" s="39"/>
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
@@ -5582,15 +5578,15 @@
       <c r="CD29" s="16"/>
     </row>
     <row r="30" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="98"/>
       <c r="D30" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="80" t="s">
+      <c r="E30" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="F30" s="86"/>
+      <c r="F30" s="92"/>
       <c r="G30" s="42" t="s">
         <v>99</v>
       </c>
@@ -5603,10 +5599,10 @@
       <c r="J30" s="7">
         <v>17</v>
       </c>
-      <c r="K30" s="80" t="s">
+      <c r="K30" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="L30" s="104"/>
+      <c r="L30" s="89"/>
       <c r="M30" s="39"/>
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
@@ -5679,15 +5675,15 @@
       <c r="CD30" s="16"/>
     </row>
     <row r="31" spans="2:82" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="100"/>
       <c r="D31" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="E31" s="78" t="s">
+      <c r="E31" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="76"/>
+      <c r="F31" s="107"/>
       <c r="G31" s="42" t="s">
         <v>152</v>
       </c>
@@ -5700,10 +5696,10 @@
       <c r="J31" s="7">
         <v>10</v>
       </c>
-      <c r="K31" s="78" t="s">
+      <c r="K31" s="90" t="s">
         <v>160</v>
       </c>
-      <c r="L31" s="133"/>
+      <c r="L31" s="91"/>
       <c r="M31" s="39"/>
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
@@ -5776,15 +5772,15 @@
       <c r="CD31" s="16"/>
     </row>
     <row r="32" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B32" s="87" t="s">
+      <c r="B32" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="88"/>
+      <c r="C32" s="96"/>
       <c r="D32" s="68">
         <v>3</v>
       </c>
-      <c r="E32" s="97"/>
-      <c r="F32" s="98"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="123"/>
       <c r="G32" s="28"/>
       <c r="H32" s="29"/>
       <c r="I32" s="32">
@@ -5795,8 +5791,8 @@
         <f>SUM(J33:J40)</f>
         <v>17</v>
       </c>
-      <c r="K32" s="95"/>
-      <c r="L32" s="99"/>
+      <c r="K32" s="116"/>
+      <c r="L32" s="111"/>
       <c r="M32" s="20"/>
       <c r="N32" s="11"/>
       <c r="O32" s="11"/>
@@ -5826,38 +5822,38 @@
       <c r="AM32" s="11"/>
       <c r="AN32" s="11"/>
       <c r="AO32" s="11"/>
-      <c r="AP32" s="115"/>
-      <c r="AQ32" s="115"/>
-      <c r="AR32" s="115"/>
-      <c r="AS32" s="115"/>
-      <c r="AT32" s="115"/>
-      <c r="AU32" s="115"/>
-      <c r="AV32" s="115"/>
-      <c r="AW32" s="115"/>
-      <c r="AX32" s="115"/>
-      <c r="AY32" s="115"/>
-      <c r="AZ32" s="115"/>
-      <c r="BA32" s="115"/>
-      <c r="BB32" s="115"/>
-      <c r="BC32" s="115"/>
-      <c r="BD32" s="115"/>
-      <c r="BE32" s="115"/>
-      <c r="BF32" s="115"/>
-      <c r="BG32" s="115"/>
-      <c r="BH32" s="115"/>
-      <c r="BI32" s="115"/>
-      <c r="BJ32" s="115"/>
-      <c r="BK32" s="115"/>
-      <c r="BL32" s="115"/>
-      <c r="BM32" s="115"/>
-      <c r="BN32" s="115"/>
-      <c r="BO32" s="115"/>
-      <c r="BP32" s="115"/>
-      <c r="BQ32" s="115"/>
-      <c r="BR32" s="115"/>
-      <c r="BS32" s="115"/>
-      <c r="BT32" s="115"/>
-      <c r="BU32" s="115"/>
+      <c r="AP32" s="70"/>
+      <c r="AQ32" s="70"/>
+      <c r="AR32" s="70"/>
+      <c r="AS32" s="70"/>
+      <c r="AT32" s="70"/>
+      <c r="AU32" s="70"/>
+      <c r="AV32" s="70"/>
+      <c r="AW32" s="70"/>
+      <c r="AX32" s="70"/>
+      <c r="AY32" s="70"/>
+      <c r="AZ32" s="70"/>
+      <c r="BA32" s="70"/>
+      <c r="BB32" s="70"/>
+      <c r="BC32" s="70"/>
+      <c r="BD32" s="70"/>
+      <c r="BE32" s="70"/>
+      <c r="BF32" s="70"/>
+      <c r="BG32" s="70"/>
+      <c r="BH32" s="70"/>
+      <c r="BI32" s="70"/>
+      <c r="BJ32" s="70"/>
+      <c r="BK32" s="70"/>
+      <c r="BL32" s="70"/>
+      <c r="BM32" s="70"/>
+      <c r="BN32" s="70"/>
+      <c r="BO32" s="70"/>
+      <c r="BP32" s="70"/>
+      <c r="BQ32" s="70"/>
+      <c r="BR32" s="70"/>
+      <c r="BS32" s="70"/>
+      <c r="BT32" s="70"/>
+      <c r="BU32" s="70"/>
       <c r="BV32" s="11"/>
       <c r="BW32" s="11"/>
       <c r="BX32" s="11"/>
@@ -5869,15 +5865,15 @@
       <c r="CD32" s="11"/>
     </row>
     <row r="33" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="98"/>
       <c r="D33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="100" t="s">
+      <c r="E33" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="100"/>
+      <c r="F33" s="109"/>
       <c r="G33" s="40" t="s">
         <v>103</v>
       </c>
@@ -5890,10 +5886,10 @@
       <c r="J33" s="26">
         <v>0</v>
       </c>
-      <c r="K33" s="100" t="s">
+      <c r="K33" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="L33" s="101"/>
+      <c r="L33" s="106"/>
       <c r="M33" s="12"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -5966,15 +5962,15 @@
       <c r="CD33" s="4"/>
     </row>
     <row r="34" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="98"/>
       <c r="D34" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="80" t="s">
+      <c r="E34" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="86"/>
+      <c r="F34" s="92"/>
       <c r="G34" s="40" t="s">
         <v>100</v>
       </c>
@@ -5987,10 +5983,10 @@
       <c r="J34" s="26">
         <v>0</v>
       </c>
-      <c r="K34" s="80" t="s">
+      <c r="K34" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="L34" s="81"/>
+      <c r="L34" s="101"/>
       <c r="M34" s="12"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -6062,15 +6058,15 @@
       <c r="CD34" s="4"/>
     </row>
     <row r="35" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="89"/>
-      <c r="C35" s="90"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="80" t="s">
+      <c r="E35" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="86"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="40" t="s">
         <v>129</v>
       </c>
@@ -6083,10 +6079,10 @@
       <c r="J35" s="26">
         <v>6</v>
       </c>
-      <c r="K35" s="80" t="s">
+      <c r="K35" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="L35" s="104"/>
+      <c r="L35" s="89"/>
       <c r="M35" s="39"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
@@ -6159,15 +6155,15 @@
       <c r="CD35" s="16"/>
     </row>
     <row r="36" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="98"/>
       <c r="D36" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="110" t="s">
+      <c r="E36" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="96"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="40" t="s">
         <v>129</v>
       </c>
@@ -6180,10 +6176,10 @@
       <c r="J36" s="26">
         <v>6</v>
       </c>
-      <c r="K36" s="80" t="s">
+      <c r="K36" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="L36" s="104"/>
+      <c r="L36" s="89"/>
       <c r="M36" s="39"/>
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
@@ -6256,15 +6252,15 @@
       <c r="CD36" s="16"/>
     </row>
     <row r="37" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="89"/>
-      <c r="C37" s="90"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="98"/>
       <c r="D37" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="80" t="s">
+      <c r="E37" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="86"/>
+      <c r="F37" s="92"/>
       <c r="G37" s="40" t="s">
         <v>125</v>
       </c>
@@ -6277,10 +6273,10 @@
       <c r="J37" s="26">
         <v>1</v>
       </c>
-      <c r="K37" s="110" t="s">
+      <c r="K37" s="93" t="s">
         <v>116</v>
       </c>
-      <c r="L37" s="81"/>
+      <c r="L37" s="101"/>
       <c r="M37" s="39"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
@@ -6353,15 +6349,15 @@
       <c r="CD37" s="16"/>
     </row>
     <row r="38" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="98"/>
       <c r="D38" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="80" t="s">
+      <c r="E38" s="88" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="86"/>
+      <c r="F38" s="92"/>
       <c r="G38" s="40" t="s">
         <v>124</v>
       </c>
@@ -6374,10 +6370,10 @@
       <c r="J38" s="7">
         <v>0</v>
       </c>
-      <c r="K38" s="85" t="s">
+      <c r="K38" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="L38" s="101"/>
+      <c r="L38" s="106"/>
       <c r="M38" s="39"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
@@ -6450,15 +6446,15 @@
       <c r="CD38" s="16"/>
     </row>
     <row r="39" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="89"/>
-      <c r="C39" s="90"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="80" t="s">
+      <c r="E39" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="86"/>
+      <c r="F39" s="92"/>
       <c r="G39" s="40" t="s">
         <v>155</v>
       </c>
@@ -6471,10 +6467,10 @@
       <c r="J39" s="7">
         <v>2</v>
       </c>
-      <c r="K39" s="85" t="s">
+      <c r="K39" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="L39" s="101"/>
+      <c r="L39" s="106"/>
       <c r="M39" s="39"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
@@ -6547,15 +6543,15 @@
       <c r="CD39" s="16"/>
     </row>
     <row r="40" spans="2:82" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="91"/>
-      <c r="C40" s="92"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="100"/>
       <c r="D40" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E40" s="78" t="s">
+      <c r="E40" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="76"/>
+      <c r="F40" s="107"/>
       <c r="G40" s="40" t="s">
         <v>130</v>
       </c>
@@ -6568,10 +6564,10 @@
       <c r="J40" s="47">
         <v>2</v>
       </c>
-      <c r="K40" s="85" t="s">
+      <c r="K40" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="L40" s="101"/>
+      <c r="L40" s="106"/>
       <c r="M40" s="13"/>
       <c r="N40" s="14"/>
       <c r="O40" s="14"/>
@@ -6644,15 +6640,15 @@
       <c r="CD40" s="14"/>
     </row>
     <row r="41" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="88"/>
+      <c r="C41" s="96"/>
       <c r="D41" s="69">
         <v>4</v>
       </c>
-      <c r="E41" s="102"/>
-      <c r="F41" s="95"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="116"/>
       <c r="G41" s="28"/>
       <c r="H41" s="29"/>
       <c r="I41" s="32">
@@ -6663,89 +6659,89 @@
         <f>SUM(J42:J48)</f>
         <v>56</v>
       </c>
-      <c r="K41" s="94"/>
-      <c r="L41" s="99"/>
+      <c r="K41" s="110"/>
+      <c r="L41" s="111"/>
       <c r="M41" s="49"/>
       <c r="N41" s="11"/>
       <c r="O41" s="11"/>
       <c r="P41" s="11"/>
-      <c r="Q41" s="115"/>
-      <c r="R41" s="115"/>
-      <c r="S41" s="115"/>
-      <c r="T41" s="115"/>
-      <c r="U41" s="115"/>
-      <c r="V41" s="115"/>
-      <c r="W41" s="115"/>
-      <c r="X41" s="115"/>
-      <c r="Y41" s="115"/>
-      <c r="Z41" s="115"/>
-      <c r="AA41" s="115"/>
-      <c r="AB41" s="115"/>
-      <c r="AC41" s="115"/>
-      <c r="AD41" s="115"/>
-      <c r="AE41" s="115"/>
-      <c r="AF41" s="115"/>
-      <c r="AG41" s="115"/>
-      <c r="AH41" s="115"/>
-      <c r="AI41" s="115"/>
-      <c r="AJ41" s="115"/>
-      <c r="AK41" s="115"/>
-      <c r="AL41" s="115"/>
-      <c r="AM41" s="115"/>
-      <c r="AN41" s="115"/>
-      <c r="AO41" s="115"/>
-      <c r="AP41" s="115"/>
-      <c r="AQ41" s="115"/>
-      <c r="AR41" s="115"/>
-      <c r="AS41" s="115"/>
-      <c r="AT41" s="115"/>
-      <c r="AU41" s="115"/>
-      <c r="AV41" s="115"/>
-      <c r="AW41" s="115"/>
-      <c r="AX41" s="115"/>
-      <c r="AY41" s="115"/>
-      <c r="AZ41" s="115"/>
-      <c r="BA41" s="115"/>
-      <c r="BB41" s="115"/>
-      <c r="BC41" s="115"/>
-      <c r="BD41" s="115"/>
-      <c r="BE41" s="115"/>
-      <c r="BF41" s="115"/>
-      <c r="BG41" s="115"/>
-      <c r="BH41" s="115"/>
-      <c r="BI41" s="115"/>
-      <c r="BJ41" s="115"/>
-      <c r="BK41" s="115"/>
-      <c r="BL41" s="115"/>
-      <c r="BM41" s="115"/>
-      <c r="BN41" s="115"/>
-      <c r="BO41" s="115"/>
-      <c r="BP41" s="115"/>
-      <c r="BQ41" s="115"/>
-      <c r="BR41" s="115"/>
-      <c r="BS41" s="115"/>
-      <c r="BT41" s="115"/>
-      <c r="BU41" s="115"/>
-      <c r="BV41" s="115"/>
-      <c r="BW41" s="115"/>
-      <c r="BX41" s="115"/>
-      <c r="BY41" s="115"/>
-      <c r="BZ41" s="115"/>
-      <c r="CA41" s="115"/>
+      <c r="Q41" s="70"/>
+      <c r="R41" s="70"/>
+      <c r="S41" s="70"/>
+      <c r="T41" s="70"/>
+      <c r="U41" s="70"/>
+      <c r="V41" s="70"/>
+      <c r="W41" s="70"/>
+      <c r="X41" s="70"/>
+      <c r="Y41" s="70"/>
+      <c r="Z41" s="70"/>
+      <c r="AA41" s="70"/>
+      <c r="AB41" s="70"/>
+      <c r="AC41" s="70"/>
+      <c r="AD41" s="70"/>
+      <c r="AE41" s="70"/>
+      <c r="AF41" s="70"/>
+      <c r="AG41" s="70"/>
+      <c r="AH41" s="70"/>
+      <c r="AI41" s="70"/>
+      <c r="AJ41" s="70"/>
+      <c r="AK41" s="70"/>
+      <c r="AL41" s="70"/>
+      <c r="AM41" s="70"/>
+      <c r="AN41" s="70"/>
+      <c r="AO41" s="70"/>
+      <c r="AP41" s="70"/>
+      <c r="AQ41" s="70"/>
+      <c r="AR41" s="70"/>
+      <c r="AS41" s="70"/>
+      <c r="AT41" s="70"/>
+      <c r="AU41" s="70"/>
+      <c r="AV41" s="70"/>
+      <c r="AW41" s="70"/>
+      <c r="AX41" s="70"/>
+      <c r="AY41" s="70"/>
+      <c r="AZ41" s="70"/>
+      <c r="BA41" s="70"/>
+      <c r="BB41" s="70"/>
+      <c r="BC41" s="70"/>
+      <c r="BD41" s="70"/>
+      <c r="BE41" s="70"/>
+      <c r="BF41" s="70"/>
+      <c r="BG41" s="70"/>
+      <c r="BH41" s="70"/>
+      <c r="BI41" s="70"/>
+      <c r="BJ41" s="70"/>
+      <c r="BK41" s="70"/>
+      <c r="BL41" s="70"/>
+      <c r="BM41" s="70"/>
+      <c r="BN41" s="70"/>
+      <c r="BO41" s="70"/>
+      <c r="BP41" s="70"/>
+      <c r="BQ41" s="70"/>
+      <c r="BR41" s="70"/>
+      <c r="BS41" s="70"/>
+      <c r="BT41" s="70"/>
+      <c r="BU41" s="70"/>
+      <c r="BV41" s="70"/>
+      <c r="BW41" s="70"/>
+      <c r="BX41" s="70"/>
+      <c r="BY41" s="70"/>
+      <c r="BZ41" s="70"/>
+      <c r="CA41" s="70"/>
       <c r="CB41" s="11"/>
       <c r="CC41" s="11"/>
       <c r="CD41" s="11"/>
     </row>
     <row r="42" spans="2:82" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="98"/>
       <c r="D42" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="86" t="s">
+      <c r="E42" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="85"/>
+      <c r="F42" s="103"/>
       <c r="G42" s="40" t="s">
         <v>156</v>
       </c>
@@ -6758,10 +6754,10 @@
       <c r="J42" s="41">
         <v>0</v>
       </c>
-      <c r="K42" s="86" t="s">
+      <c r="K42" s="92" t="s">
         <v>163</v>
       </c>
-      <c r="L42" s="101"/>
+      <c r="L42" s="106"/>
       <c r="M42" s="18"/>
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
@@ -6834,19 +6830,19 @@
       <c r="CD42" s="16"/>
     </row>
     <row r="43" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="98"/>
       <c r="D43" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="80" t="s">
+      <c r="E43" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="86"/>
-      <c r="G43" s="117">
+      <c r="F43" s="92"/>
+      <c r="G43" s="72">
         <v>45786</v>
       </c>
-      <c r="H43" s="118">
+      <c r="H43" s="73">
         <v>45848</v>
       </c>
       <c r="I43" s="6">
@@ -6855,10 +6851,10 @@
       <c r="J43" s="41">
         <v>48</v>
       </c>
-      <c r="K43" s="93" t="s">
+      <c r="K43" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="L43" s="81"/>
+      <c r="L43" s="101"/>
       <c r="M43" s="5"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -6931,15 +6927,15 @@
       <c r="CD43" s="4"/>
     </row>
     <row r="44" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B44" s="89"/>
-      <c r="C44" s="90"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="98"/>
       <c r="D44" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="80" t="s">
+      <c r="E44" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="F44" s="86"/>
+      <c r="F44" s="92"/>
       <c r="G44" s="43" t="s">
         <v>158</v>
       </c>
@@ -6952,10 +6948,10 @@
       <c r="J44" s="41">
         <v>3</v>
       </c>
-      <c r="K44" s="93" t="s">
+      <c r="K44" s="115" t="s">
         <v>164</v>
       </c>
-      <c r="L44" s="81"/>
+      <c r="L44" s="101"/>
       <c r="M44" s="5"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -7028,15 +7024,15 @@
       <c r="CD44" s="4"/>
     </row>
     <row r="45" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B45" s="89"/>
-      <c r="C45" s="90"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="98"/>
       <c r="D45" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="80" t="s">
+      <c r="E45" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="93"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="44" t="s">
         <v>156</v>
       </c>
@@ -7049,10 +7045,10 @@
       <c r="J45" s="41">
         <v>1</v>
       </c>
-      <c r="K45" s="93" t="s">
+      <c r="K45" s="115" t="s">
         <v>135</v>
       </c>
-      <c r="L45" s="104"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="5"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
@@ -7125,15 +7121,15 @@
       <c r="CD45" s="4"/>
     </row>
     <row r="46" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="98"/>
       <c r="D46" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="80" t="s">
+      <c r="E46" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="F46" s="86"/>
+      <c r="F46" s="92"/>
       <c r="G46" s="43" t="s">
         <v>124</v>
       </c>
@@ -7146,10 +7142,10 @@
       <c r="J46" s="41">
         <v>0</v>
       </c>
-      <c r="K46" s="107" t="s">
+      <c r="K46" s="112" t="s">
         <v>116</v>
       </c>
-      <c r="L46" s="81"/>
+      <c r="L46" s="101"/>
       <c r="M46" s="5"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -7222,15 +7218,15 @@
       <c r="CD46" s="4"/>
     </row>
     <row r="47" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B47" s="89"/>
-      <c r="C47" s="90"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="98"/>
       <c r="D47" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="80" t="s">
+      <c r="E47" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="F47" s="86"/>
+      <c r="F47" s="92"/>
       <c r="G47" s="43" t="s">
         <v>108</v>
       </c>
@@ -7243,10 +7239,10 @@
       <c r="J47" s="41">
         <v>0</v>
       </c>
-      <c r="K47" s="107" t="s">
+      <c r="K47" s="112" t="s">
         <v>116</v>
       </c>
-      <c r="L47" s="81"/>
+      <c r="L47" s="101"/>
       <c r="M47" s="5"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -7319,15 +7315,15 @@
       <c r="CD47" s="4"/>
     </row>
     <row r="48" spans="2:82" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="91"/>
-      <c r="C48" s="92"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="100"/>
       <c r="D48" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E48" s="78" t="s">
+      <c r="E48" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="76"/>
+      <c r="F48" s="107"/>
       <c r="G48" s="43" t="s">
         <v>158</v>
       </c>
@@ -7340,10 +7336,10 @@
       <c r="J48" s="47">
         <v>4</v>
       </c>
-      <c r="K48" s="109" t="s">
+      <c r="K48" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="L48" s="79"/>
+      <c r="L48" s="114"/>
       <c r="M48" s="15"/>
       <c r="N48" s="14"/>
       <c r="O48" s="14"/>
@@ -7416,15 +7412,15 @@
       <c r="CD48" s="14"/>
     </row>
     <row r="49" spans="2:82" x14ac:dyDescent="0.2">
-      <c r="B49" s="87" t="s">
+      <c r="B49" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="88"/>
+      <c r="C49" s="96"/>
       <c r="D49" s="69">
         <v>5</v>
       </c>
-      <c r="E49" s="102"/>
-      <c r="F49" s="103"/>
+      <c r="E49" s="119"/>
+      <c r="F49" s="120"/>
       <c r="G49" s="28"/>
       <c r="H49" s="29"/>
       <c r="I49" s="32">
@@ -7435,8 +7431,8 @@
         <f>SUM(J50:J55)</f>
         <v>0</v>
       </c>
-      <c r="K49" s="105"/>
-      <c r="L49" s="106"/>
+      <c r="K49" s="117"/>
+      <c r="L49" s="118"/>
       <c r="M49" s="50"/>
       <c r="N49" s="48"/>
       <c r="O49" s="48"/>
@@ -7500,24 +7496,24 @@
       <c r="BU49" s="48"/>
       <c r="BV49" s="48"/>
       <c r="BW49" s="48"/>
-      <c r="BX49" s="116"/>
-      <c r="BY49" s="116"/>
-      <c r="BZ49" s="116"/>
-      <c r="CA49" s="116"/>
-      <c r="CB49" s="116"/>
+      <c r="BX49" s="71"/>
+      <c r="BY49" s="71"/>
+      <c r="BZ49" s="71"/>
+      <c r="CA49" s="71"/>
+      <c r="CB49" s="71"/>
       <c r="CC49" s="48"/>
       <c r="CD49" s="48"/>
     </row>
     <row r="50" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="89"/>
-      <c r="C50" s="90"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="98"/>
       <c r="D50" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="86" t="s">
+      <c r="E50" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="F50" s="85"/>
+      <c r="F50" s="103"/>
       <c r="G50" s="40" t="s">
         <v>113</v>
       </c>
@@ -7530,10 +7526,10 @@
       <c r="J50" s="41">
         <v>0</v>
       </c>
-      <c r="K50" s="86" t="s">
+      <c r="K50" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="L50" s="101"/>
+      <c r="L50" s="106"/>
       <c r="M50" s="19"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
@@ -7606,15 +7602,15 @@
       <c r="CD50" s="4"/>
     </row>
     <row r="51" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="97"/>
+      <c r="C51" s="98"/>
       <c r="D51" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="80" t="s">
+      <c r="E51" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="96"/>
+      <c r="F51" s="94"/>
       <c r="G51" s="44" t="s">
         <v>108</v>
       </c>
@@ -7627,10 +7623,10 @@
       <c r="J51" s="41">
         <v>0</v>
       </c>
-      <c r="K51" s="93" t="s">
+      <c r="K51" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="L51" s="81"/>
+      <c r="L51" s="101"/>
       <c r="M51" s="18"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
@@ -7703,15 +7699,15 @@
       <c r="CD51" s="16"/>
     </row>
     <row r="52" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="98"/>
       <c r="D52" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="80" t="s">
+      <c r="E52" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="F52" s="86"/>
+      <c r="F52" s="92"/>
       <c r="G52" s="40" t="s">
         <v>108</v>
       </c>
@@ -7724,10 +7720,10 @@
       <c r="J52" s="41">
         <v>0</v>
       </c>
-      <c r="K52" s="93" t="s">
+      <c r="K52" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="L52" s="81"/>
+      <c r="L52" s="101"/>
       <c r="M52" s="18"/>
       <c r="N52" s="16"/>
       <c r="O52" s="16"/>
@@ -7800,15 +7796,15 @@
       <c r="CD52" s="16"/>
     </row>
     <row r="53" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="89"/>
-      <c r="C53" s="90"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="98"/>
       <c r="D53" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="80" t="s">
+      <c r="E53" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="F53" s="86"/>
+      <c r="F53" s="92"/>
       <c r="G53" s="40" t="s">
         <v>127</v>
       </c>
@@ -7821,10 +7817,10 @@
       <c r="J53" s="41">
         <v>0</v>
       </c>
-      <c r="K53" s="93" t="s">
+      <c r="K53" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="L53" s="81"/>
+      <c r="L53" s="101"/>
       <c r="M53" s="18"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
@@ -7897,15 +7893,15 @@
       <c r="CD53" s="16"/>
     </row>
     <row r="54" spans="2:82" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="89"/>
-      <c r="C54" s="90"/>
+      <c r="B54" s="97"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="80" t="s">
+      <c r="E54" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="F54" s="96"/>
+      <c r="F54" s="94"/>
       <c r="G54" s="44" t="s">
         <v>114</v>
       </c>
@@ -7918,10 +7914,10 @@
       <c r="J54" s="41">
         <v>0</v>
       </c>
-      <c r="K54" s="93" t="s">
+      <c r="K54" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="L54" s="81"/>
+      <c r="L54" s="101"/>
       <c r="M54" s="18"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
@@ -7994,15 +7990,15 @@
       <c r="CD54" s="16"/>
     </row>
     <row r="55" spans="2:82" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="91"/>
-      <c r="C55" s="92"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="100"/>
       <c r="D55" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E55" s="86" t="s">
+      <c r="E55" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="F55" s="85"/>
+      <c r="F55" s="103"/>
       <c r="G55" s="40" t="s">
         <v>114</v>
       </c>
@@ -8015,7 +8011,7 @@
       <c r="J55" s="41">
         <v>0</v>
       </c>
-      <c r="K55" s="76" t="s">
+      <c r="K55" s="107" t="s">
         <v>31</v>
       </c>
       <c r="L55" s="108"/>
@@ -8092,25 +8088,41 @@
     </row>
   </sheetData>
   <mergeCells count="105">
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B49:C55"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="B13:C20"/>
-    <mergeCell ref="B21:C31"/>
-    <mergeCell ref="B32:C40"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M9:S9"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B41:C48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="BX9:CD9"/>
+    <mergeCell ref="T9:Z9"/>
+    <mergeCell ref="AA9:AG9"/>
+    <mergeCell ref="AH9:AN9"/>
+    <mergeCell ref="AO9:AU9"/>
+    <mergeCell ref="AV9:BB9"/>
+    <mergeCell ref="BC9:BI9"/>
+    <mergeCell ref="BJ9:BP9"/>
+    <mergeCell ref="BQ9:BW9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="K50:L50"/>
@@ -8135,10 +8147,40 @@
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="B13:C20"/>
+    <mergeCell ref="B21:C31"/>
+    <mergeCell ref="B32:C40"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="K38:L38"/>
     <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B49:C55"/>
     <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K29:L29"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E44:F44"/>
@@ -8151,52 +8193,6 @@
     <mergeCell ref="E51:F51"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E50:F50"/>
-    <mergeCell ref="BX9:CD9"/>
-    <mergeCell ref="T9:Z9"/>
-    <mergeCell ref="AA9:AG9"/>
-    <mergeCell ref="AH9:AN9"/>
-    <mergeCell ref="AO9:AU9"/>
-    <mergeCell ref="AV9:BB9"/>
-    <mergeCell ref="BC9:BI9"/>
-    <mergeCell ref="BJ9:BP9"/>
-    <mergeCell ref="BQ9:BW9"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B41:C48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M9:S9"/>
-    <mergeCell ref="B1:L2"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8235,17 +8231,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="133" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
     </row>
     <row r="2" spans="1:9" ht="285" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="66"/>

</xml_diff>